<commit_message>
Bed Ownership Tools 업데이트
#2303
</commit_message>
<xml_diff>
--- a/Data/Bed Ownership Tools - 3558407174/3558407174.xlsx
+++ b/Data/Bed Ownership Tools - 3558407174/3558407174.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Main_250907" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Main_251002" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="379">
   <si>
     <t xml:space="preserve">Class+Node [(Identifier (Key)]</t>
   </si>
@@ -439,18 +439,6 @@
     <t xml:space="preserve">활성화하면 침대 소유자 지정 창에 모든 맵, 상단, 그리고 교통수단에 있는 정착민이 표시됩니다. 비활성화하면 바닐라와 같이 해당 침대가 있는 맵에 있는 정착민만 표시합니다.</t>
   </si>
   <si>
-    <t xml:space="preserve">Keyed+BedOwnershipTools.EnableHospitalityModCompatPatches</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BedOwnershipTools.EnableHospitalityModCompatPatches</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enable Hospitality mod compatibility patches</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hospitality 모드 호환성 패치 활성화</t>
-  </si>
-  <si>
     <t xml:space="preserve">Keyed+BedOwnershipTools.EnableModCompatPatches_Tooltip</t>
   </si>
   <si>
@@ -650,6 +638,525 @@
   </si>
   <si>
     <t xml:space="preserve">(비활성)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.AlertNeedAutoDeathrestBuildingPawn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.AlertNeedAutoDeathrestBuildingPawn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{PAWN} cannot auto-deathrest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{PAWN}(이)가 자동 죽음안식 불가</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.AlertNeedAutoDeathrestBuildingPawns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.AlertNeedAutoDeathrestBuildingPawns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{NUMCULPRITS} colonists cannot auto-deathrest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{NUMCULPRITS}명의 정착민이 자동 죽음안식 불가</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.AlertNeedAutoDeathrestBuildingDesc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.AlertNeedAutoDeathrestBuildingDesc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A colonist is unable to automatically deathrest.\n\nTo fix this, ensure that the colonist can reach {ANACCEPTABLEDEATHRESTBUILDING}.\n\nThese people need {ANACCEPTABLEDEATHRESTBUILDING}:\n{CULPRITS}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">자동 죽음안식이 불가능한 정착민이 있습니다.\n\n해당 정착민이 {ANACCEPTABLEDEATHRESTBUILDING}에 접근 가능하도록 하십시오.\n\n다음 정착민이 {ANACCEPTABLEDEATHRESTBUILDING}(을)를 필요로 합니다:\n{CULPRITS}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.AnAssignedBedOrDeathrestCasket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.AnAssignedBedOrDeathrestCasket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a bed or assigned deathrest casket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">침대 또는 지정된 죽음안식 관</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.AnAssignedDeathrestCasket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.AnAssignedDeathrestCasket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">an assigned deathrest casket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">지정된 죽음안식 관</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.Command_SetAutomaticDeathrestMode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.Command_SetAutomaticDeathrestMode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto-d.rest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">자동 죽음안식</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.Command_SetAutomaticDeathrestModeDesc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.Command_SetAutomaticDeathrestModeDesc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set a schedule that {PAWN_nameDef} will follow for automatic deathrest.\n\nCurrent schedule: {SCHEDULE}\n\n{SCHEDULEDESC}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{PAWN_nameDef}(이)가 자동 죽음안식 시 따를 일정을 설정합니다.\n\n현재 일정: {SCHEDULE}\n\n{SCHEDULEDESC}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.Command_SetAutomaticDeathrestModeManualScheduleDesc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.Command_SetAutomaticDeathrestModeManualScheduleDesc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{PAWN_nameDef} will only deathrest if ordered to do so.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{PAWN_nameDef}(은)는 자동으로 죽음안식에 들지 않을 것입니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.Command_SetAutomaticDeathrestModeExhaustionScheduleDesc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.Command_SetAutomaticDeathrestModeExhaustionScheduleDesc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{PAWN_nameDef} will attempt to deathrest in the scheduled time before exhaustion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{PAWN_nameDef}(은)는 탈진까지 일정 시간이 남으면 죽음안식에 들려 시도할 것입니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.Command_SetAutomaticDeathrestModeCalendarScheduleDesc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.Command_SetAutomaticDeathrestModeCalendarScheduleDesc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{PAWN_nameDef} will attempt to deathrest at the scheduled times of year, or if {PAWN_pronoun} is near exhaustion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{PAWN_nameDef}(은)는 정해진 날짜 동안, 혹은 탈진 상태에 가까워졌을 때 죽음안식에 들려 시도할 것입니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.Command_UnbindDeathrestBindable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.Command_UnbindDeathrestBindable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unbind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">종속 해제</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.Command_UnbindDeathrestBindableDesc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.Command_UnbindDeathrestBindableDesc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unbind this building's user.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">이 건물이 주인에게 더 이상 종속되지 않게 합니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.Command_UnbindDeathrestBindableDisabledNoBindeeReason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.Command_UnbindDeathrestBindableDisabledNoBindeeReason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This building is not currently bound.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">이 건물은 현재 종속되지 않았습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.Command_GenericDisabledDesc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.Command_GenericDisabledDesc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This command is unavailable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">이 명령은 현재 사용 불가능합니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.Command_GenericDisabledNoOwnerReason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.Command_GenericDisabledNoOwnerReason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This building does not have a valid assigned or bound deathrester.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">이 건물은 유효한 소유자에게 지정 또는 종속되지 않았습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.Command_AutoWakeDisabledCalendarReason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.Command_AutoWakeDisabledCalendarReason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colonists following calendar deathrest schedules will always auto-wake.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">정해진 날짜 동안 죽음안식에 들도록 설정된 정착민은 항상 자동으로 기상합니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.CommunalBedsHeading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.CommunalBedsHeading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communal beds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">공용 침대</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.AssignmentPinningHeading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.AssignmentPinningHeading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assignment pinning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.AssignmentGroupsHeading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.AssignmentGroupsHeading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assignment groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.DeathrestBindingsHeading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.DeathrestBindingsHeading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deathrest bindings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">죽음안식 종속</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.AutomaticDeathrestHeading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.AutomaticDeathrestHeading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automatic deathrest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.UICustomizationsHeading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.UICustomizationsHeading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI customizations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI 커스터마이징</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.ModCompatibilityHeading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.ModCompatibilityHeading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mod compatibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">모드 호환성</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.DeveloperSettingsHeading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.DeveloperSettingsHeading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Developer settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">개발자 설정</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.ResetSettingsButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.ResetSettingsButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reset settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">설정 초기화</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.ResetDeveloperSettingsButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.ResetDeveloperSettingsButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[DEV] Reset developer settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[DEV] 개발자 설정 초기화</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.EnableSpareDeathrestBindings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.EnableSpareDeathrestBindings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable spare deathrest bindings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">여러 죽음안식 건물 종속 가능</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.EnableSpareDeathrestBindings_Tooltip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.EnableSpareDeathrestBindings_Tooltip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If enabled, deathresters can bind to multiple deathrest caskets and more buildings than supported by their deathrest serum capacity.\n\nWith spare bindings, deathresters can switch between deathrest buildings without needing to deconstruct the previously used set. Deathresters will still be limited by serum capacity while deathresting.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">활성화하면 죽음안식이 가능한 정착민이 여러 개의 죽음안식 관을 종속해 죽음안식 수용량보다 더 많은 수의 장치와 연결할 수 있습니다.\n\n이 기능을 사용하면 이전에 사용하던 죽음안식 시설을 해체하지 않고도 여러 죽음안식 건물을 사용할 수 있습니다. 죽음안식 중에는 여전히 죽음안식 수용량의 제한을 받습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.DeathrestBindingsArePermanent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.DeathrestBindingsArePermanent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deathrest bindings are permanent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">영구적인 죽음안식 종속</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.DeathrestBindingsArePermanent_Tooltip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.DeathrestBindingsArePermanent_Tooltip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If enabled with the spare deathrest bindings feature, retains vanilla game behaviour where deathrest buildings are irreversibly bound to the building's first user. If disabled, allows bound buildings to be transferred between deathresters without restriction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">여러 죽음안식 건물 종속 기능과 함께 활성화할 경우, 바닐라 설정을 따라 죽음안식 건물이 첫 사용자에게 영구적으로 종속됩니다. 비활성화하면 이미 종속된 죽음안식 건물이라도 제한 없이 주인을 바꿀 수 있게 됩니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.EnableAutomaticDeathrest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.EnableAutomaticDeathrest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable automatic deathrest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">자동 죽음안식 활성화</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.EnableAutomaticDeathrest_Tooltip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.EnableAutomaticDeathrest_Tooltip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If enabled, allows the player to optionally assign automatic deathrest schedules to deathrester colonists.\n\nDeathresters following a schedule will autonomously deathrest on certain calendar dates or at certain exhaustion levels. Deathresters will not automatically deathrest if they do not own a deathrest casket or regular bed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">활성화 시 죽음안식이 가능한 정착민의 자동 죽음안식 일정을 설정할 수 있게 됩니다.\n\n죽음안식이 가능한 정착민이 정해진 일정에 따르도록 하면 특정 날짜나 탈진까지 남은 시간에 따라 자동으로 죽음안식에 듭니다. 죽음안식 관 또는 일반 침대를 소유하지 않은 정착민은 자동 죽음안식에 들지 않습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.IgnoreBedsForAutomaticDeathrest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.IgnoreBedsForAutomaticDeathrest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ignore beds for automatic deathrest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">자동 죽음안식 시 침대 사용 금지</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.IgnoreBedsForAutomaticDeathrest_Tooltip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.IgnoreBedsForAutomaticDeathrest_Tooltip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If enabled with the automatic deathrest feature, deathrester colonists will not use regular beds for automatic deathrest. If disabled, deathrester colonists will consider using regular beds for automatic deathrest if they cannot locate a deathrest casket.\n\nDeathresters will always prioritize using deathrest caskets over beds.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">자동 죽음안식 기능과 함께 활성화하면 죽음안식이 가능한 정착민들이 침대에서 자동 죽음안식을 하지 않습니다. 비활성화하면 죽음안식 관을 찾지 못할 경우 일반 침대에서 자동 죽음안식에 들려 시도합니다.\n\n죽음안식 관은 항상 침대보다 더 높은 우선순위를 가집니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.HideDeathrestAutoControlsOnPawnWhileAwake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.HideDeathrestAutoControlsOnPawnWhileAwake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hide deathrest auto-controls on pawn while awake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">깨어 있는 동안 자동 죽음안식 설정 숨기기</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.HideDeathrestAutoControlsOnPawnWhileAwake_Tooltip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.HideDeathrestAutoControlsOnPawnWhileAwake_Tooltip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If enabled, deathrester colonists will only expose deathrest scheduling and auto-wake controls while deathresting. If disabled, always shows deathrest controls when such pawns are selected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">활성화하면 자동 죽음안식 일정 및 자동 기상 설정이 죽음안식 중일 때에만 표시됩니다. 비활성화하면 죽음안식이 가능한 정착민을 선택했을 때 해당 설정을 항상 표시합니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.ShowDeathrestAutoControlsOnCasket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.ShowDeathrestAutoControlsOnCasket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show deathrest auto-controls on deathrest caskets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">죽음안식 관에 자동 죽음안식 설정 표시</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.ShowDeathrestAutoControlsOnCasket_Tooltip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.ShowDeathrestAutoControlsOnCasket_Tooltip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If enabled, deathrest caskets will expose deathrest scheduling and auto-wake controls associated with their bound pawn. If disabled, only the pawn will expose such settings.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">활성화하면 죽음안식 관에 주인의 자동 죽음안식 일정 및 자동 기상 설정을 표시합니다. 비활성화하면 폰 선택 시에만 해당 설정을 표시합니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.EnableModCompatPatches</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.EnableModCompatPatches</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable "{0}" support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"{0}" 호환 기능 활성화</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.DevEnableExtraMenusAndGizmos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.DevEnableExtraMenusAndGizmos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[DEV] Enable extra menus and gizmos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[DEV] 추가 메뉴 및 버튼 활성화</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.DevEnableExtraMenusAndGizmos_Tooltip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.DevEnableExtraMenusAndGizmos_Tooltip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enables extra developer menus and gizmos in game, to assist with testing the mod.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">모드를 테스트하기 위한 추가적인 개발자 메뉴와 버튼을 활성화합니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.ScheduleManual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.ScheduleManual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">수동</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.ScheduleTimePeriodBeforeExhaustion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.ScheduleTimePeriodBeforeExhaustion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{0} before exhaustion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">탈진까지 {0} 남았을 때</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyed+BedOwnershipTools.ScheduleBiannualDateRange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BedOwnershipTools.ScheduleBiannualDateRange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2}/{3} ({0}-{1})</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{2}/{3} ({0}일-{1}일)</t>
   </si>
 </sst>
 </file>
@@ -690,12 +1197,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF87CEEB"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -732,12 +1245,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -750,6 +1267,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF87CEEB"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -933,24 +1510,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F42" activeCellId="0" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.6328125" defaultRowHeight="16.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="16.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="68.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="62.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="48.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="68.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="62.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="48.13"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="1" width="7.63"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -970,7 +1547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -987,7 +1564,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1004,7 +1581,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -1021,7 +1598,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -1038,7 +1615,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1055,7 +1632,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -1072,7 +1649,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -1089,7 +1666,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -1106,7 +1683,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
@@ -1123,7 +1700,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>43</v>
       </c>
@@ -1140,7 +1717,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>47</v>
       </c>
@@ -1157,7 +1734,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
@@ -1174,7 +1751,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
@@ -1191,7 +1768,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>59</v>
       </c>
@@ -1208,7 +1785,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>63</v>
       </c>
@@ -1225,7 +1802,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>67</v>
       </c>
@@ -1242,7 +1819,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>71</v>
       </c>
@@ -1259,7 +1836,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>75</v>
       </c>
@@ -1276,7 +1853,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>79</v>
       </c>
@@ -1293,7 +1870,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>83</v>
       </c>
@@ -1310,7 +1887,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>87</v>
       </c>
@@ -1327,7 +1904,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>91</v>
       </c>
@@ -1344,7 +1921,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>95</v>
       </c>
@@ -1361,7 +1938,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>99</v>
       </c>
@@ -1378,7 +1955,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>103</v>
       </c>
@@ -1395,7 +1972,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>107</v>
       </c>
@@ -1412,7 +1989,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>111</v>
       </c>
@@ -1429,7 +2006,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>115</v>
       </c>
@@ -1446,7 +2023,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>119</v>
       </c>
@@ -1463,7 +2040,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>123</v>
       </c>
@@ -1480,7 +2057,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>127</v>
       </c>
@@ -1497,7 +2074,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>131</v>
       </c>
@@ -1514,7 +2091,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>135</v>
       </c>
@@ -1531,7 +2108,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>139</v>
       </c>
@@ -1548,7 +2125,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>143</v>
       </c>
@@ -1565,7 +2142,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>147</v>
       </c>
@@ -1582,7 +2159,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>151</v>
       </c>
@@ -1599,7 +2176,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>155</v>
       </c>
@@ -1616,7 +2193,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>159</v>
       </c>
@@ -1633,7 +2210,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>163</v>
       </c>
@@ -1647,27 +2224,27 @@
         <v>165</v>
       </c>
       <c r="F41" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
+      <c r="B42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="43" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>170</v>
       </c>
@@ -1684,7 +2261,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>174</v>
       </c>
@@ -1701,7 +2278,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>178</v>
       </c>
@@ -1718,7 +2295,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>182</v>
       </c>
@@ -1735,7 +2312,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>186</v>
       </c>
@@ -1752,7 +2329,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>190</v>
       </c>
@@ -1769,7 +2346,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>194</v>
       </c>
@@ -1786,7 +2363,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>198</v>
       </c>
@@ -1803,7 +2380,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>202</v>
       </c>
@@ -1830,11 +2407,742 @@
       <c r="C52" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E52" s="2" t="s">
         <v>208</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>209</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>